<commit_message>
add check naming sheets
</commit_message>
<xml_diff>
--- a/exampleexcel.xlsx
+++ b/exampleexcel.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Лист2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="first" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="second" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -292,13 +292,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>500.0</v>
       </c>
     </row>
@@ -318,11 +318,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>1337.0</v>
       </c>
       <c r="B1" s="1">
-        <v>100.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="2">
@@ -330,39 +330,39 @@
         <v>1337.0</v>
       </c>
       <c r="B2" s="1">
-        <v>-200.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1337.0</v>
       </c>
       <c r="B3" s="1">
-        <v>-300.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
-        <v>1337.0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2000.0</v>
+      <c r="A4" s="1">
+        <v>1337.0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-30.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>1337.0</v>
       </c>
       <c r="B5" s="1">
-        <v>3000.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>1337.0</v>
       </c>
       <c r="B6" s="1">
-        <v>-1000.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="7">
@@ -370,7 +370,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="1">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="8">
@@ -378,7 +378,7 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1">
-        <v>-20.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="9">
@@ -386,7 +386,7 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="1">
-        <v>30.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="10">
@@ -394,7 +394,7 @@
         <v>1.0</v>
       </c>
       <c r="B10" s="1">
-        <v>40.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="11">
@@ -402,7 +402,31 @@
         <v>1.0</v>
       </c>
       <c r="B11" s="1">
-        <v>50.0</v>
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-300.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>400.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>